<commit_message>
changes to intro i guess
</commit_message>
<xml_diff>
--- a/scripts/lbunits_conjugate.xlsx
+++ b/scripts/lbunits_conjugate.xlsx
@@ -1293,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMI80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1"/>
@@ -8799,7 +8799,7 @@
       <c r="E25" s="32"/>
       <c r="F25" s="4">
         <f>dt/dx</f>
-        <v>5.0000000000000001E-3</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>109</v>
@@ -10939,7 +10939,7 @@
       <c r="D32" s="9"/>
       <c r="E32" s="33"/>
       <c r="F32" s="40">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="G32" s="3">
         <f>dx^2</f>
@@ -12065,7 +12065,7 @@
       <c r="E38" s="33"/>
       <c r="F38" s="9">
         <f>(dt/dx^2)*(1/nsRe)</f>
-        <v>0.29599999999999987</v>
+        <v>2.9599999999999991E-2</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>54</v>
@@ -12090,7 +12090,7 @@
       <c r="E39" s="33"/>
       <c r="F39" s="9">
         <f>nu/latticeC+0.5</f>
-        <v>1.3879999999999997</v>
+        <v>0.58879999999999999</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -12112,7 +12112,7 @@
       <c r="E40" s="34"/>
       <c r="F40" s="11">
         <f>1/nstau</f>
-        <v>0.72046109510086476</v>
+        <v>1.6983695652173914</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -12135,7 +12135,7 @@
       <c r="E41" s="33"/>
       <c r="F41" s="9">
         <f>(dt/dx^2) * (1/nsPe)</f>
-        <v>0.44643982553715283</v>
+        <v>4.4643982553715288E-2</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -12157,7 +12157,7 @@
       <c r="E42" s="33"/>
       <c r="F42" s="9">
         <f>alpha/thermalLatticeC+0.5</f>
-        <v>2.2857593021486116</v>
+        <v>0.67857593021486118</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -12178,7 +12178,7 @@
       <c r="E43" s="34"/>
       <c r="F43" s="11">
         <f>1/adtau</f>
-        <v>0.43749138374281182</v>
+        <v>1.4736744341688697</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -16397,7 +16397,7 @@
       <c r="E54" s="33"/>
       <c r="F54" s="9">
         <f>(dt/dx^2)*(1/cjPe)</f>
-        <v>0.1337209302325581</v>
+        <v>1.3372093023255812E-2</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -16415,7 +16415,7 @@
       <c r="E55" s="33"/>
       <c r="F55" s="9">
         <f>cjNu/thermalLatticeC+0.5</f>
-        <v>1.0348837209302324</v>
+        <v>0.55348837209302326</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
@@ -16433,7 +16433,7 @@
       <c r="E56" s="34"/>
       <c r="F56" s="11">
         <f>1/cjTau</f>
-        <v>0.96629213483146081</v>
+        <v>1.8067226890756303</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
@@ -16512,7 +16512,7 @@
       </c>
       <c r="D63" s="2">
         <f xml:space="preserve"> ( P_res_i / 3 ) * Rho0 * dx^2 / dt^2</f>
-        <v>107413.33333333337</v>
+        <v>10741333.333333338</v>
       </c>
       <c r="E63" s="28" t="s">
         <v>78</v>
@@ -16527,7 +16527,7 @@
       </c>
       <c r="D64" s="2">
         <f xml:space="preserve"> ( P_res_o / 3 ) * Rho0 * dx^2 / dt^2</f>
-        <v>1066.6666666666667</v>
+        <v>106666.66666666667</v>
       </c>
       <c r="E64" s="28" t="s">
         <v>78</v>
@@ -16542,7 +16542,7 @@
       </c>
       <c r="D65" s="41">
         <f>D63-D64</f>
-        <v>106346.6666666667</v>
+        <v>10634666.666666672</v>
       </c>
       <c r="E65" s="28" t="s">
         <v>78</v>
@@ -16651,7 +16651,7 @@
       </c>
       <c r="F76" s="38">
         <f>D76/uD*uLB</f>
-        <v>5.0000000000000001E-3</v>
+        <v>5.0000000000000001E-4</v>
       </c>
     </row>
     <row r="77" spans="2:11" ht="16.5" customHeight="1">

</xml_diff>